<commit_message>
pivot small fixes (#17)
</commit_message>
<xml_diff>
--- a/tests/Templates/tPivot1.xlsx
+++ b/tests/Templates/tPivot1.xlsx
@@ -148,7 +148,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +171,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="43"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9F7CFF"/>
+        <bgColor indexed="42"/>
       </patternFill>
     </fill>
   </fills>
@@ -202,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -210,8 +216,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -248,6 +252,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -268,52 +275,39 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>590550</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="1695450" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3075" name="Picture 2" descr="I:\Images\4\bmpLogo4.gif"/>
+        <xdr:cNvPr id="3" name="Рисунок 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="2390775" y="19050"/>
-          <a:ext cx="2228850" cy="571500"/>
+          <a:off x="2933700" y="0"/>
+          <a:ext cx="1695450" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -672,7 +666,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -682,15 +676,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.25" customHeight="1">
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
@@ -698,48 +693,48 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="30.75" customHeight="1">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -750,7 +745,7 @@
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -770,13 +765,13 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="17"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>